<commit_message>
auto eval + game changes
</commit_message>
<xml_diff>
--- a/Auto-Eval-ASI2-r1.xlsx
+++ b/Auto-Eval-ASI2-r1.xlsx
@@ -525,12 +525,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="104">
     <dxf>
@@ -1332,19 +1332,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L44" activeCellId="0" sqref="L44"/>
+      <selection pane="topLeft" activeCell="I34" activeCellId="0" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,7 +1538,7 @@
       <c r="Q6" s="14"/>
       <c r="R6" s="14"/>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="21" t="s">
@@ -1552,13 +1554,13 @@
         <v>13</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="J7" s="23" t="s">
         <v>14</v>
@@ -1579,7 +1581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="21" t="s">
@@ -1595,13 +1597,13 @@
         <v>13</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>16</v>
       </c>
       <c r="J8" s="23" t="s">
         <v>16</v>
@@ -1622,7 +1624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="21" t="s">
@@ -1638,13 +1640,13 @@
         <v>13</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>16</v>
       </c>
       <c r="J9" s="23" t="s">
         <v>16</v>
@@ -1665,7 +1667,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="21" t="s">
@@ -1683,11 +1685,11 @@
       <c r="G10" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>20</v>
+      <c r="H10" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>16</v>
       </c>
       <c r="J10" s="23" t="s">
         <v>16</v>
@@ -1708,7 +1710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="20.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="21.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="21" t="s">
@@ -1724,13 +1726,13 @@
         <v>13</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="J11" s="23" t="s">
         <v>14</v>
@@ -1751,7 +1753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="20.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="21.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="21" t="s">
@@ -1767,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>16</v>
       </c>
       <c r="J12" s="23" t="s">
         <v>14</v>
@@ -1794,7 +1796,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="21" t="s">
@@ -1810,13 +1812,13 @@
         <v>13</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="J13" s="23" t="s">
         <v>14</v>
@@ -1837,7 +1839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="21.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="21" t="s">
@@ -1853,13 +1855,13 @@
         <v>13</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="J14" s="23" t="s">
         <v>14</v>
@@ -1880,7 +1882,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="21" t="s">
@@ -1896,13 +1898,13 @@
         <v>13</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="J15" s="23" t="s">
         <v>16</v>
@@ -1923,7 +1925,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="20.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="21.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="21" t="s">
@@ -1939,13 +1941,13 @@
         <v>13</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>16</v>
       </c>
       <c r="J16" s="23" t="s">
         <v>16</v>
@@ -1966,7 +1968,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="21" t="s">
@@ -1982,13 +1984,13 @@
         <v>13</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="J17" s="23" t="s">
         <v>14</v>
@@ -2009,7 +2011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="20.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="21" t="s">
@@ -2025,13 +2027,13 @@
         <v>13</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="J18" s="23" t="s">
         <v>16</v>
@@ -2052,7 +2054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="20.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="21.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="21" t="s">
@@ -2068,13 +2070,13 @@
         <v>13</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="J19" s="23" t="s">
         <v>14</v>
@@ -2095,7 +2097,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="20.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="21" t="s">
@@ -2111,13 +2113,13 @@
         <v>13</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="J20" s="23" t="s">
         <v>16</v>
@@ -2138,7 +2140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="20.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="21" t="s">
@@ -2154,13 +2156,13 @@
         <v>13</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>16</v>
       </c>
       <c r="J21" s="23" t="s">
         <v>14</v>
@@ -2181,7 +2183,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="21" t="s">
@@ -2197,13 +2199,13 @@
         <v>13</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>16</v>
       </c>
       <c r="J22" s="23" t="s">
         <v>28</v>
@@ -2224,7 +2226,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="20.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="21.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="21" t="s">
@@ -2240,13 +2242,13 @@
         <v>13</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="J23" s="23" t="s">
         <v>14</v>
@@ -2267,7 +2269,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="20.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="21" t="s">
@@ -2283,13 +2285,13 @@
         <v>13</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>16</v>
       </c>
       <c r="J24" s="23" t="s">
         <v>14</v>
@@ -2326,22 +2328,22 @@
         <v>13</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L25" s="25" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M25" s="23" t="s">
         <v>14</v>
@@ -3114,7 +3116,7 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B26:C26"/>
   </mergeCells>
-  <conditionalFormatting sqref="D27:E41 D7:E25 G7:H25 G27:H41 J27:K41 J10:J25 M7:N25 M27:N40 M41:O41 O37:O40 J7:K9 K10:K25">
+  <conditionalFormatting sqref="D27:E41 D7:E25 G27:H41 J27:K41 J10:J25 M7:N25 M27:N40 M41:O41 O37:O40 J7:K9 K10:K25">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"A"</formula>
     </cfRule>
@@ -3242,7 +3244,7 @@
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27:I41 I7:I25">
+  <conditionalFormatting sqref="I27:I41">
     <cfRule type="cellIs" priority="40" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
       <formula>"A"</formula>
     </cfRule>
@@ -3484,15 +3486,1335 @@
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" priority="108" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="109" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="110" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="111" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="112" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="113" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="cellIs" priority="114" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="115" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="116" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="117" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="118" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="119" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" priority="120" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="121" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="122" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="123" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="124" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="125" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="cellIs" priority="126" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="127" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="128" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="129" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="130" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="131" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="cellIs" priority="132" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="133" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="134" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="135" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="136" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="137" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" priority="138" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="139" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="140" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="141" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="142" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="143" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20">
+    <cfRule type="cellIs" priority="144" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="145" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="146" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="147" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="148" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="149" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="cellIs" priority="150" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="151" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="152" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="153" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="154" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="155" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="cellIs" priority="156" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="157" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="158" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="159" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="160" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="161" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25">
+    <cfRule type="cellIs" priority="162" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="163" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="164" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="165" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="166" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="167" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" priority="168" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="169" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="170" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="171" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="172" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="173" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="cellIs" priority="174" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="175" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="176" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="177" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="178" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="179" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="cellIs" priority="180" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="181" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="182" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="183" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="184" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="185" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="cellIs" priority="186" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="187" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="188" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="189" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="190" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="191" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="cellIs" priority="192" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="193" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="194" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="195" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="196" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="197" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="cellIs" priority="198" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="199" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="200" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="201" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="202" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="203" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="cellIs" priority="204" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="205" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="206" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="207" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="208" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="209" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" priority="210" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="211" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="212" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="213" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="214" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="215" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" priority="216" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="217" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="218" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="219" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="220" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="221" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="cellIs" priority="222" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="223" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="224" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="225" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="226" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="227" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" priority="228" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="229" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="230" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="231" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="232" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="233" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" priority="234" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="235" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="236" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="237" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="238" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="239" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" priority="240" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="241" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="242" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="243" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="244" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="245" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" priority="246" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="247" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="248" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="249" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="250" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="251" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="cellIs" priority="252" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="253" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="254" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="255" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="256" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="257" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="cellIs" priority="258" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="259" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="260" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="261" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="262" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="263" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="cellIs" priority="264" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="265" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="266" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="267" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="268" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="269" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="cellIs" priority="270" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="271" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="272" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="273" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="274" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="275" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="cellIs" priority="276" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="277" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="278" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="279" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="280" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="281" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="cellIs" priority="282" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="283" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="284" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="285" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="286" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="287" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" priority="288" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="289" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="290" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="291" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="292" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="293" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" priority="294" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="295" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="296" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="297" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="298" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="299" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="cellIs" priority="300" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="301" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="302" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="303" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="304" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="305" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" priority="306" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="307" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="308" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="309" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="310" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="311" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" priority="312" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="313" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="314" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="315" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="316" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="317" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" priority="318" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="319" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="320" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="321" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="322" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="323" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" priority="324" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="325" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="326" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="327" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="328" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="329" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" priority="330" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="331" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="332" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="333" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="334" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="335" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" priority="336" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="337" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="338" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="339" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="340" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="341" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="cellIs" priority="342" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="343" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="344" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="345" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="346" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="347" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="cellIs" priority="348" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="349" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="350" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="351" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="352" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="353" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="cellIs" priority="354" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="355" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="356" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="357" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="358" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="359" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="cellIs" priority="360" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="361" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="362" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="363" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="364" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="365" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="cellIs" priority="366" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="367" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="368" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="369" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="370" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="371" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="cellIs" priority="372" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="373" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="374" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="375" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="376" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="377" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="cellIs" priority="378" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="379" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="380" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="381" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="382" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="383" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="cellIs" priority="384" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="385" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="386" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="387" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="388" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="389" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="cellIs" priority="390" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="391" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="392" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="393" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="394" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="395" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="cellIs" priority="396" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="397" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="398" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="399" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="400" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="401" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="cellIs" priority="402" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="403" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="404" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="405" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="406" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="407" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="cellIs" priority="408" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="409" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="410" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="411" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="412" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="413" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" priority="414" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="415" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="416" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="417" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="418" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="419" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="cellIs" priority="420" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="421" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="422" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="423" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="424" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="425" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" priority="426" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="427" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="428" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="429" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="430" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="431" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="cellIs" priority="432" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="433" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="434" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="435" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="436" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="437" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="cellIs" priority="438" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="439" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="440" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="441" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="442" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="443" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" priority="444" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="445" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="446" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="447" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="448" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="449" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19">
+    <cfRule type="cellIs" priority="450" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="451" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="452" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="453" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="454" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="455" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="cellIs" priority="456" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="457" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="458" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="459" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="460" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="461" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="cellIs" priority="462" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="463" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="464" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="465" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="466" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="467" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21">
+    <cfRule type="cellIs" priority="468" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="469" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="470" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="471" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="472" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="473" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22">
+    <cfRule type="cellIs" priority="474" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="475" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="476" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="477" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="478" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="479" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="cellIs" priority="480" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="481" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="482" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="483" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="484" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="485" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="cellIs" priority="486" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="487" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="488" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="489" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="490" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="491" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="cellIs" priority="492" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="493" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="494" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="495" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="496" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="497" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="cellIs" priority="498" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="499" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="500" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="501" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="502" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="503" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D7:O25 D27:O43" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D7:O25 D27:O43" type="list">
       <formula1>Note</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3502,7 +4824,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3512,57 +4834,60 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.91"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="22" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="22" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="A6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Fichiers pour rendu tp2
</commit_message>
<xml_diff>
--- a/Auto-Eval-ASI2-r1.xlsx
+++ b/Auto-Eval-ASI2-r1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c.vanden-hende\Documents\Personnel\ASI2\ASI-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD493DE-079C-4177-B5BB-A5CBC66F5DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83FD2CF-A00B-4327-BBDB-18C622F088DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="60">
   <si>
     <t>Bertrand Pautet</t>
   </si>
@@ -395,39 +395,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -435,111 +419,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="608">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAC090"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAC090"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="596">
     <dxf>
       <fill>
         <patternFill>
@@ -5304,1869 +5210,1514 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="3" customWidth="1"/>
     <col min="4" max="1025" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="3" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="3" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="9" t="s">
+      <c r="K1" s="22"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="3" t="s">
+      <c r="N1" s="1"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="19">
+      <c r="C4" s="21"/>
+      <c r="D4" s="12">
         <v>0.25</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="12">
+        <v>0.33</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13">
         <v>0.25</v>
       </c>
-      <c r="F4" s="19">
+      <c r="H4" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13">
         <v>0.25</v>
       </c>
-      <c r="G4" s="20">
+      <c r="K4" s="12">
+        <v>0.33</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="13">
         <v>0.25</v>
       </c>
-      <c r="H4" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="I4" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="J4" s="20">
-        <v>0.25</v>
-      </c>
-      <c r="K4" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="L4" s="22">
-        <v>0.25</v>
-      </c>
-      <c r="M4" s="20">
-        <v>0.25</v>
-      </c>
-      <c r="N4" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="O4" s="22">
-        <v>0.25</v>
-      </c>
-      <c r="P4" s="20">
+      <c r="N4" s="12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O4" s="14"/>
+      <c r="P4" s="13">
         <f>D4+G4+J4+M4</f>
         <v>1</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="Q4" s="12">
         <f>E4+H4+K4+N4</f>
         <v>1</v>
       </c>
-      <c r="R4" s="21">
+      <c r="R4" s="12">
         <f>F4+I4+L4+O4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="23" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="18"/>
+      <c r="M7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="18"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="23" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O8" s="27" t="s">
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="18"/>
+      <c r="M8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="23" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O9" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="18"/>
+      <c r="M9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="23" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="N10" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="27" t="s">
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="18"/>
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="23" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N11" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O11" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="18"/>
+      <c r="M11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="18"/>
     </row>
     <row r="12" spans="1:18" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="23" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M12" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" s="27" t="s">
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="18"/>
+      <c r="M12" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="23" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N13" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="18"/>
+      <c r="M13" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="18"/>
     </row>
     <row r="14" spans="1:18" ht="36.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="23" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M14" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N14" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="18"/>
+      <c r="M14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="18"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="23" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M15" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N15" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O15" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="18"/>
+      <c r="M15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="18"/>
     </row>
     <row r="16" spans="1:18" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="23" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L16" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M16" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="N16" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O16" s="27" t="s">
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="18"/>
+      <c r="M16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="23" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M17" s="26" t="s">
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="18"/>
+      <c r="M17" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="N17" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O17" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="N17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O17" s="18"/>
     </row>
     <row r="18" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="23" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K18" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L18" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M18" s="26" t="s">
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="18"/>
+      <c r="M18" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O18" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="N18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O18" s="18"/>
     </row>
     <row r="19" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="23" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="25" t="s">
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M19" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N19" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O19" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="18"/>
+      <c r="M19" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N19" t="s">
+        <v>16</v>
+      </c>
+      <c r="O19" s="18"/>
     </row>
     <row r="20" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="23" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K20" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L20" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M20" s="26" t="s">
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="16"/>
+      <c r="J20" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="18"/>
+      <c r="M20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="N20" s="27" t="s">
+      <c r="N20" t="s">
         <v>28</v>
       </c>
-      <c r="O20" s="28" t="s">
-        <v>28</v>
-      </c>
+      <c r="O20" s="18"/>
     </row>
     <row r="21" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="23" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M21" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N21" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O21" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="16"/>
+      <c r="J21" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="18"/>
+      <c r="M21" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" t="s">
+        <v>16</v>
+      </c>
+      <c r="O21" s="18"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="23" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="25" t="s">
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="25" t="s">
+      <c r="I22" s="16"/>
+      <c r="J22" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="K22" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="L22" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="M22" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N22" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O22" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="L22" s="18"/>
+      <c r="M22" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O22" s="18"/>
     </row>
     <row r="23" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="23" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K23" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M23" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N23" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O23" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="16"/>
+      <c r="J23" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="18"/>
+      <c r="M23" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N23" t="s">
+        <v>14</v>
+      </c>
+      <c r="O23" s="18"/>
     </row>
     <row r="24" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="23" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L24" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M24" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N24" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O24" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="16"/>
+      <c r="J24" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" s="18"/>
+      <c r="M24" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" s="18"/>
     </row>
     <row r="25" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="23" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="25" t="s">
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="H25" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L25" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N25" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O25" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="I25" s="16"/>
+      <c r="J25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="18"/>
+      <c r="M25" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" s="18"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="18"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="11"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="23" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K27" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L27" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M27" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N27" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O27" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="18"/>
+      <c r="M27" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N27" t="s">
+        <v>14</v>
+      </c>
+      <c r="O27" s="18"/>
     </row>
     <row r="28" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="23" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K28" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L28" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M28" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N28" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O28" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="18"/>
+      <c r="M28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O28" s="18"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="23" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K29" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M29" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N29" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O29" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K29" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="18"/>
+      <c r="M29" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" t="s">
+        <v>14</v>
+      </c>
+      <c r="O29" s="18"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="23" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K30" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L30" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M30" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O30" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="18"/>
+      <c r="M30" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" t="s">
+        <v>16</v>
+      </c>
+      <c r="O30" s="18"/>
     </row>
     <row r="31" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="23" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="26" t="s">
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="K31" s="27" t="s">
+      <c r="K31" t="s">
         <v>28</v>
       </c>
-      <c r="L31" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="M31" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N31" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O31" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="L31" s="18"/>
+      <c r="M31" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N31" t="s">
+        <v>16</v>
+      </c>
+      <c r="O31" s="18"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="23" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D32" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K32" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M32" s="26" t="s">
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="18"/>
+      <c r="M32" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N32" s="27" t="s">
+      <c r="N32" t="s">
         <v>28</v>
       </c>
-      <c r="O32" s="28" t="s">
-        <v>28</v>
-      </c>
+      <c r="O32" s="18"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="23" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K33" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L33" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M33" s="26" t="s">
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" t="s">
+        <v>14</v>
+      </c>
+      <c r="L33" s="18"/>
+      <c r="M33" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N33" s="27" t="s">
+      <c r="N33" t="s">
         <v>28</v>
       </c>
-      <c r="O33" s="28" t="s">
-        <v>28</v>
-      </c>
+      <c r="O33" s="18"/>
     </row>
     <row r="34" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="23" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D34" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="26" t="s">
+      <c r="E34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H34" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="J34" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K34" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L34" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M34" s="26" t="s">
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K34" t="s">
+        <v>14</v>
+      </c>
+      <c r="L34" s="18"/>
+      <c r="M34" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N34" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O34" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="N34" t="s">
+        <v>16</v>
+      </c>
+      <c r="O34" s="18"/>
     </row>
     <row r="35" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="23" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="26" t="s">
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H35" s="27" t="s">
+      <c r="H35" t="s">
         <v>28</v>
       </c>
-      <c r="I35" s="27" t="s">
+      <c r="J35" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" s="18"/>
+      <c r="M35" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N35" t="s">
         <v>28</v>
       </c>
-      <c r="J35" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K35" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L35" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="M35" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="N35" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="O35" s="28" t="s">
-        <v>28</v>
-      </c>
+      <c r="O35" s="18"/>
     </row>
     <row r="36" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="23" t="s">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="26" t="s">
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="K36" s="27" t="s">
+      <c r="K36" t="s">
         <v>28</v>
       </c>
-      <c r="L36" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="M36" s="26" t="s">
+      <c r="L36" s="18"/>
+      <c r="M36" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N36" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O36" s="28" t="s">
-        <v>28</v>
-      </c>
+      <c r="N36" t="s">
+        <v>16</v>
+      </c>
+      <c r="O36" s="18"/>
     </row>
     <row r="37" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="23" t="s">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D37" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="26" t="s">
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H37" s="27" t="s">
+      <c r="H37" t="s">
         <v>28</v>
       </c>
-      <c r="I37" s="27" t="s">
+      <c r="J37" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" t="s">
         <v>28</v>
       </c>
-      <c r="J37" s="26" t="s">
+      <c r="L37" s="18"/>
+      <c r="M37" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K37" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="L37" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="M37" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="N37" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="O37" s="27" t="s">
+      <c r="N37" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="23" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="24" t="s">
+      <c r="D38" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="26" t="s">
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H38" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="26" t="s">
+      <c r="H38" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="K38" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L38" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M38" s="26" t="s">
+      <c r="K38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38" s="18"/>
+      <c r="M38" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N38" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O38" s="27" t="s">
+      <c r="N38" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="23" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="24" t="s">
+      <c r="D39" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" t="s">
         <v>28</v>
       </c>
-      <c r="F39" s="24" t="s">
+      <c r="G39" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G39" s="26" t="s">
+      <c r="K39" t="s">
+        <v>28</v>
+      </c>
+      <c r="L39" s="18"/>
+      <c r="M39" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H39" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="K39" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="L39" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="M39" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="N39" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="O39" s="27" t="s">
+      <c r="N39" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="23" t="s">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="24" t="s">
+      <c r="D40" t="s">
         <v>20</v>
       </c>
-      <c r="E40" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="26" t="s">
+      <c r="E40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H40" s="27" t="s">
+      <c r="H40" t="s">
         <v>28</v>
       </c>
-      <c r="I40" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="26" t="s">
+      <c r="J40" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="K40" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L40" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M40" s="26" t="s">
+      <c r="K40" t="s">
+        <v>16</v>
+      </c>
+      <c r="L40" s="18"/>
+      <c r="M40" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N40" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="O40" s="27" t="s">
+      <c r="N40" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="23" t="s">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="J41" s="26" t="s">
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="18"/>
+      <c r="J41" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="K41" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L41" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M41" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N41" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="O41" s="26" t="s">
-        <v>16</v>
-      </c>
+      <c r="K41" t="s">
+        <v>16</v>
+      </c>
+      <c r="L41" s="18"/>
+      <c r="M41" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O41" s="17"/>
     </row>
     <row r="42" spans="1:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="23" t="s">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L42" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="O42" s="26" t="s">
-        <v>16</v>
-      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="18"/>
+      <c r="J42" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" t="s">
+        <v>16</v>
+      </c>
+      <c r="L42" s="18"/>
+      <c r="M42" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O42" s="17"/>
     </row>
     <row r="43" spans="1:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="23" t="s">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="26" t="s">
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H43" s="27" t="s">
+      <c r="H43" t="s">
         <v>28</v>
       </c>
-      <c r="I43" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="J43" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L43" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="M43" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N43" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="O43" s="26" t="s">
-        <v>16</v>
-      </c>
+      <c r="J43" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" t="s">
+        <v>16</v>
+      </c>
+      <c r="L43" s="18"/>
+      <c r="M43" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O43" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="G34:H40 J27:K41 M7:N25 M27:N40 M41:O41 O37:O40 J7:K25 G27:H27 G29:H30 D7:E18 D19:F25 D27:F41">
-    <cfRule type="cellIs" dxfId="607" priority="14" operator="equal">
-      <formula>"A"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="606" priority="15" operator="equal">
-      <formula>"AB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="605" priority="16" operator="equal">
-      <formula>"B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="604" priority="17" operator="equal">
-      <formula>"C"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="603" priority="18" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="602" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="595" priority="14" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="594" priority="15" operator="equal">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="593" priority="16" operator="equal">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="592" priority="17" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="591" priority="18" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="590" priority="19" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42:K42 M42:O42 D42:F42">
-    <cfRule type="cellIs" dxfId="601" priority="20" operator="equal">
-      <formula>"A"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="600" priority="21" operator="equal">
-      <formula>"AB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="599" priority="22" operator="equal">
-      <formula>"B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="598" priority="23" operator="equal">
-      <formula>"C"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="597" priority="24" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="596" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="589" priority="20" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="588" priority="21" operator="equal">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="587" priority="22" operator="equal">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="586" priority="23" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="585" priority="24" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="584" priority="25" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43:K43 M43:O43 D43:H43">
-    <cfRule type="cellIs" dxfId="595" priority="26" operator="equal">
-      <formula>"A"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="594" priority="27" operator="equal">
-      <formula>"AB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="593" priority="28" operator="equal">
-      <formula>"B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="592" priority="29" operator="equal">
-      <formula>"C"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="591" priority="30" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="590" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="583" priority="26" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="582" priority="27" operator="equal">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="581" priority="28" operator="equal">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="580" priority="29" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="579" priority="30" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="578" priority="31" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:R4">
-    <cfRule type="cellIs" dxfId="589" priority="32" operator="notEqual">
+    <cfRule type="cellIs" dxfId="577" priority="32" operator="notEqual">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="588" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="576" priority="33" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F14 F16:F17">
-    <cfRule type="cellIs" dxfId="587" priority="34" operator="equal">
-      <formula>"A"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="586" priority="35" operator="equal">
-      <formula>"AB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="585" priority="36" operator="equal">
-      <formula>"B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="584" priority="37" operator="equal">
-      <formula>"C"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="583" priority="38" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="582" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="575" priority="34" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="574" priority="35" operator="equal">
+      <formula>"AB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="573" priority="36" operator="equal">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="572" priority="37" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="571" priority="38" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="570" priority="39" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9119,47 +8670,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="24" t="s">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="24" t="s">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>